<commit_message>
Corretti errori campi in checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#HEALTHSTRATEGYXX/HealthStrategy/HEasy/49.00.00/report-checklist.xlsx
+++ b/GATEWAY/A1#111#HEALTHSTRATEGYXX/HealthStrategy/HEasy/49.00.00/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthstrategysrl.sharepoint.com/sites/Operations/Shared Documents/Integrazioni/_Documentazione generale/FSE2/Nazionale/Finalizzazione Accreditamento Nazionale/A1#111#HEALTHSTRATEGYXX__HealthStrategy__HEasy__49.00.00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Bagatta\Downloads\it-fse-accreditamento-health-strategy-main\it-fse-accreditamento-health-strategy-main\GATEWAY\A1#111#HEALTHSTRATEGYXX\HealthStrategy\HEasy\49.00.00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="13_ncr:1_{8A964438-CA3D-403A-94DB-61DD83690133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB0B123D-8F47-46DA-B04F-541F2D5CC095}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD58F28B-361D-4577-BA41-3361A0430E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="338" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="533">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1996,6 +1996,9 @@
   </si>
   <si>
     <t>Errore di sintassi. - ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
+  </si>
+  <si>
+    <t>Si è verificato un timeout. Si prega di riprovare a breve.</t>
   </si>
 </sst>
 </file>
@@ -2912,8 +2915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,18 +4065,18 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J192" sqref="J192"/>
+      <selection pane="bottomRight" activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
     <col min="6" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
@@ -5212,7 +5215,9 @@
       <c r="G31" s="37"/>
       <c r="H31" s="37"/>
       <c r="I31" s="42"/>
-      <c r="J31" s="38"/>
+      <c r="J31" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K31" s="38"/>
       <c r="L31" s="38"/>
       <c r="M31" s="38" t="s">
@@ -5221,8 +5226,12 @@
       <c r="N31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="38"/>
-      <c r="P31" s="38"/>
+      <c r="O31" s="38" t="s">
+        <v>532</v>
+      </c>
+      <c r="P31" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="Q31" s="38" t="s">
         <v>66</v>
       </c>
@@ -17997,26 +18006,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e52759eb-aa63-4575-955d-0abf9e6fcf9f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010022E7AE48B492574CABEFAF3718F51D73" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7008baeff8a27f72ad2af446011d87e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8" xmlns:ns3="e52759eb-aa63-4575-955d-0abf9e6fcf9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="350d21349dd8377ed54b1dcb8a90b1bc" ns2:_="" ns3:_="">
     <xsd:import namespace="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8"/>
@@ -18217,26 +18206,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e52759eb-aa63-4575-955d-0abf9e6fcf9f"/>
-    <ds:schemaRef ds:uri="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e52759eb-aa63-4575-955d-0abf9e6fcf9f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64DF73C5-1B60-4BEA-A20B-9E7C7D1EA206}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18255,6 +18245,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e52759eb-aa63-4575-955d-0abf9e6fcf9f"/>
+    <ds:schemaRef ds:uri="91cd1685-7ea0-4eb7-9574-de7dbd81b8b8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>